<commit_message>
Both -1 and -11 are doomed :-(
</commit_message>
<xml_diff>
--- a/SWE2_A08ex/manualTest.xlsx
+++ b/SWE2_A08ex/manualTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="28">
   <si>
     <t>A</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>ix</t>
+  </si>
+  <si>
+    <t>testGetValidPositions2</t>
+  </si>
+  <si>
+    <t>testGetValidPositions</t>
   </si>
 </sst>
 </file>
@@ -109,12 +115,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,11 +141,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,18 +448,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Y99"/>
+  <dimension ref="A1:AC100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AJ8" sqref="AJ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="15" max="15" width="4.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -475,8 +497,36 @@
       <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="T3" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -487,8 +537,18 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -499,8 +559,18 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U5" s="1">
+        <v>2</v>
+      </c>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -511,8 +581,18 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U6" s="1">
+        <v>3</v>
+      </c>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -527,8 +607,22 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U7" s="1">
+        <v>4</v>
+      </c>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -543,8 +637,22 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U8" s="1">
+        <v>5</v>
+      </c>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -555,8 +663,18 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U9" s="1">
+        <v>6</v>
+      </c>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>7</v>
       </c>
@@ -567,8 +685,18 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U10" s="1">
+        <v>7</v>
+      </c>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>8</v>
       </c>
@@ -579,8 +707,18 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U11" s="1">
+        <v>8</v>
+      </c>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -609,8 +747,36 @@
       <c r="J14" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="T14" t="s">
+        <v>18</v>
+      </c>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>1</v>
       </c>
@@ -621,8 +787,18 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U15" s="1">
+        <v>1</v>
+      </c>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>2</v>
       </c>
@@ -633,8 +809,18 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U16" s="1">
+        <v>2</v>
+      </c>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>3</v>
       </c>
@@ -645,8 +831,18 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U17" s="1">
+        <v>3</v>
+      </c>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>4</v>
       </c>
@@ -663,8 +859,24 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U18" s="1">
+        <v>4</v>
+      </c>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>5</v>
       </c>
@@ -679,8 +891,22 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U19" s="1">
+        <v>5</v>
+      </c>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>6</v>
       </c>
@@ -691,8 +917,18 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U20" s="1">
+        <v>6</v>
+      </c>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>7</v>
       </c>
@@ -703,8 +939,18 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U21" s="1">
+        <v>7</v>
+      </c>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>8</v>
       </c>
@@ -715,8 +961,18 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U22" s="1">
+        <v>8</v>
+      </c>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -745,8 +1001,36 @@
       <c r="J25" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="T25" t="s">
+        <v>18</v>
+      </c>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC25" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>1</v>
       </c>
@@ -757,8 +1041,18 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U26" s="1">
+        <v>1</v>
+      </c>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>2</v>
       </c>
@@ -769,8 +1063,18 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U27" s="1">
+        <v>2</v>
+      </c>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>3</v>
       </c>
@@ -783,8 +1087,20 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U28" s="1">
+        <v>3</v>
+      </c>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>4</v>
       </c>
@@ -801,8 +1117,24 @@
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U29" s="1">
+        <v>4</v>
+      </c>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>5</v>
       </c>
@@ -817,8 +1149,22 @@
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U30" s="1">
+        <v>5</v>
+      </c>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>6</v>
       </c>
@@ -829,8 +1175,18 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U31" s="1">
+        <v>6</v>
+      </c>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>7</v>
       </c>
@@ -841,8 +1197,18 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U32" s="1">
+        <v>7</v>
+      </c>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>8</v>
       </c>
@@ -853,8 +1219,18 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U33" s="1">
+        <v>8</v>
+      </c>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -883,8 +1259,36 @@
       <c r="J36" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="T36" t="s">
+        <v>19</v>
+      </c>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC36" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>1</v>
       </c>
@@ -895,8 +1299,18 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U37" s="1">
+        <v>1</v>
+      </c>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="1"/>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>2</v>
       </c>
@@ -907,8 +1321,20 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U38" s="1">
+        <v>2</v>
+      </c>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB38" s="1"/>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>3</v>
       </c>
@@ -923,8 +1349,20 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U39" s="1">
+        <v>3</v>
+      </c>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA39" s="1"/>
+      <c r="AB39" s="1"/>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>4</v>
       </c>
@@ -941,8 +1379,24 @@
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U40" s="1">
+        <v>4</v>
+      </c>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA40" s="1"/>
+      <c r="AB40" s="1"/>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>5</v>
       </c>
@@ -957,8 +1411,22 @@
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U41" s="1">
+        <v>5</v>
+      </c>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+      <c r="Y41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA41" s="1"/>
+      <c r="AB41" s="1"/>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <v>6</v>
       </c>
@@ -969,8 +1437,18 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U42" s="1">
+        <v>6</v>
+      </c>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+      <c r="Y42" s="1"/>
+      <c r="Z42" s="1"/>
+      <c r="AA42" s="1"/>
+      <c r="AB42" s="1"/>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
         <v>7</v>
       </c>
@@ -981,8 +1459,18 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U43" s="1">
+        <v>7</v>
+      </c>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+      <c r="Y43" s="1"/>
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="1"/>
+      <c r="AB43" s="1"/>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
         <v>8</v>
       </c>
@@ -993,8 +1481,18 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U44" s="1">
+        <v>8</v>
+      </c>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+      <c r="Y44" s="1"/>
+      <c r="Z44" s="1"/>
+      <c r="AA44" s="1"/>
+      <c r="AB44" s="1"/>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>21</v>
       </c>
@@ -1023,8 +1521,36 @@
       <c r="J47" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="T47" t="s">
+        <v>20</v>
+      </c>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC47" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
         <v>1</v>
       </c>
@@ -1035,8 +1561,18 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U48" s="1">
+        <v>1</v>
+      </c>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+      <c r="Y48" s="1"/>
+      <c r="Z48" s="1"/>
+      <c r="AA48" s="1"/>
+      <c r="AB48" s="1"/>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>2</v>
       </c>
@@ -1047,8 +1583,20 @@
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U49" s="1">
+        <v>2</v>
+      </c>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
+      <c r="X49" s="1"/>
+      <c r="Y49" s="1"/>
+      <c r="Z49" s="1"/>
+      <c r="AA49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB49" s="1"/>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B50" s="1">
         <v>3</v>
       </c>
@@ -1065,8 +1613,20 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U50" s="1">
+        <v>3</v>
+      </c>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+      <c r="X50" s="1"/>
+      <c r="Y50" s="1"/>
+      <c r="Z50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="1"/>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B51" s="1">
         <v>4</v>
       </c>
@@ -1083,8 +1643,24 @@
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U51" s="1">
+        <v>4</v>
+      </c>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA51" s="1"/>
+      <c r="AB51" s="1"/>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <v>5</v>
       </c>
@@ -1099,8 +1675,22 @@
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U52" s="1">
+        <v>5</v>
+      </c>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+      <c r="Y52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA52" s="1"/>
+      <c r="AB52" s="1"/>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
         <v>6</v>
       </c>
@@ -1111,8 +1701,18 @@
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U53" s="1">
+        <v>6</v>
+      </c>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+      <c r="Y53" s="1"/>
+      <c r="Z53" s="1"/>
+      <c r="AA53" s="1"/>
+      <c r="AB53" s="1"/>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B54" s="1">
         <v>7</v>
       </c>
@@ -1123,8 +1723,18 @@
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U54" s="1">
+        <v>7</v>
+      </c>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="X54" s="1"/>
+      <c r="Y54" s="1"/>
+      <c r="Z54" s="1"/>
+      <c r="AA54" s="1"/>
+      <c r="AB54" s="1"/>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
         <v>8</v>
       </c>
@@ -1135,8 +1745,18 @@
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="U55" s="1">
+        <v>8</v>
+      </c>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
+      <c r="X55" s="1"/>
+      <c r="Y55" s="1"/>
+      <c r="Z55" s="1"/>
+      <c r="AA55" s="1"/>
+      <c r="AB55" s="1"/>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>22</v>
       </c>
@@ -1166,7 +1786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B59" s="1">
         <v>1</v>
       </c>
@@ -1178,7 +1798,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B60" s="1">
         <v>2</v>
       </c>
@@ -1192,7 +1812,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B61" s="1">
         <v>3</v>
       </c>
@@ -1210,7 +1830,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B62" s="1">
         <v>4</v>
       </c>
@@ -1228,7 +1848,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B63" s="1">
         <v>5</v>
       </c>
@@ -1244,7 +1864,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B64" s="1">
         <v>6</v>
       </c>
@@ -1456,7 +2076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B81" s="1">
         <v>1</v>
       </c>
@@ -1470,7 +2090,7 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B82" s="1">
         <v>2</v>
       </c>
@@ -1484,7 +2104,7 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B83" s="1">
         <v>3</v>
       </c>
@@ -1502,7 +2122,7 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B84" s="1">
         <v>4</v>
       </c>
@@ -1520,7 +2140,7 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B85" s="1">
         <v>5</v>
       </c>
@@ -1538,7 +2158,7 @@
       </c>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B86" s="1">
         <v>6</v>
       </c>
@@ -1550,7 +2170,7 @@
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B87" s="1">
         <v>7</v>
       </c>
@@ -1562,7 +2182,7 @@
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B88" s="1">
         <v>8</v>
       </c>
@@ -1574,7 +2194,7 @@
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>25</v>
       </c>
@@ -1604,7 +2224,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B92" s="1">
         <v>1</v>
       </c>
@@ -1618,7 +2238,7 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B93" s="1">
         <v>2</v>
       </c>
@@ -1632,7 +2252,7 @@
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B94" s="1">
         <v>3</v>
       </c>
@@ -1651,17 +2271,8 @@
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
-      <c r="V94" t="s">
-        <v>10</v>
-      </c>
-      <c r="W94" t="s">
-        <v>11</v>
-      </c>
-      <c r="X94" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B95" s="1">
         <v>4</v>
       </c>
@@ -1680,20 +2291,8 @@
         <v>8</v>
       </c>
       <c r="I95" s="1"/>
-      <c r="V95" t="s">
-        <v>12</v>
-      </c>
-      <c r="W95" t="s">
-        <v>13</v>
-      </c>
-      <c r="X95" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y95" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B96" s="1">
         <v>5</v>
       </c>
@@ -1742,10 +2341,29 @@
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
-      <c r="I99" s="1"/>
+      <c r="F99" t="s">
+        <v>10</v>
+      </c>
+      <c r="G99" t="s">
+        <v>11</v>
+      </c>
+      <c r="H99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F100" t="s">
+        <v>12</v>
+      </c>
+      <c r="G100" t="s">
+        <v>13</v>
+      </c>
+      <c r="H100" t="s">
+        <v>14</v>
+      </c>
+      <c r="I100" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>